<commit_message>
added JW and Bible Text
</commit_message>
<xml_diff>
--- a/Bible - NT.xlsx
+++ b/Bible - NT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>English</t>
   </si>
@@ -55,6 +55,18 @@
   </si>
   <si>
     <t>Verse</t>
+  </si>
+  <si>
+    <t>Ci Kerode olwoŋo luryeko i muŋ, guniaŋe kun gititte kare ma lakalatwe onen iye</t>
+  </si>
+  <si>
+    <t>Ka doŋ ocwalogi me cito i Jerucalem kun waco botgi ni, “Wuciti wupeny lok kom latin man maber kikore, ce ka wunoŋe ci wudwokka lok, wek an bene acit awore.”</t>
+  </si>
+  <si>
+    <t>I kare ma doŋ guwinyo lok pa kabaka, gucito ki yogi ci guneno lakalatwe ma yam koŋ guneno yo tuŋ wokceŋ ca otelo nyimgi, obino ocuŋ ki malo wa i kabedo ka ma onoŋo latin-nu tye iye</t>
+  </si>
+  <si>
+    <t>Ka guneno lakalatwe meno, cwinygi obedo yom adada.</t>
   </si>
 </sst>
 </file>
@@ -406,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -481,6 +493,35 @@
         <v>2</v>
       </c>
     </row>
+    <row r="7" spans="1:3" ht="30">
+      <c r="A7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="45">
+      <c r="A8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="45">
+      <c r="A9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
collected Mathew 1 and 2
</commit_message>
<xml_diff>
--- a/Bible - NT.xlsx
+++ b/Bible - NT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
   <si>
     <t>English</t>
   </si>
@@ -24,56 +24,461 @@
     <t>Adhola</t>
   </si>
   <si>
-    <t>Magi aye gubedo kwaro Yecu Kricito, Lakwar Daudi, lakwar Abraim</t>
-  </si>
-  <si>
     <t>A record of the genealogy of Jesus Christ the son of David, the son of Abraham</t>
   </si>
   <si>
-    <t>After Jesus was born in Bethlehem in Judea, during the time of King Herod, Magi from the east came to Jerusalemand asked, “Where is the one who has been born king of the Jews? We saw his star in the east and have come to worship him.”</t>
-  </si>
-  <si>
-    <t>Ka doŋ ginywalo Yecu i Beterekem ma i Judaya i kare me loc pa kabaka Kerode, nen, luryeko mogo ma gua yo tuŋ wokceŋ gubino i Jerucalem, kun gipenyo ni,“En latin ma ginywalo me bedo kabaka pa Lujudaya-ni tye kwene? Pien onoŋo waneno lakalatwene yo tuŋ wokceŋ, ci man wabino ka wore.”</t>
-  </si>
-  <si>
-    <t>I kare ma kabaka Kerode owinyo lok man, cwinye opoto matek, kadi wa jo Jerucalem bene ducu cwinygi opoto matek</t>
-  </si>
-  <si>
-    <t>pi meno omiyo kabaka Kerode ocoko ajwagi madito ki lupwony-cik me rokgi ducu, ci openyogi ni, “Kricito mono gibinywalo kwene?”</t>
-  </si>
-  <si>
     <t>When King Herod heard this he was disturbed, and all Jerusalem with him</t>
   </si>
   <si>
     <t>When he had called together all the people's chief priests and teachers of the law, he asked them where the Christ was to be born</t>
   </si>
   <si>
-    <t>Jo-nu gudokke iye ni, “I Beterekem ma i Judaya, pien lanebi yam ocoyo ni,</t>
-  </si>
-  <si>
-    <t>They replied, “In Bethlehem in Judea, for this is what the prophet has written:</t>
-  </si>
-  <si>
     <t>Verse</t>
   </si>
   <si>
-    <t>Ci Kerode olwoŋo luryeko i muŋ, guniaŋe kun gititte kare ma lakalatwe onen iye</t>
-  </si>
-  <si>
-    <t>Ka doŋ ocwalogi me cito i Jerucalem kun waco botgi ni, “Wuciti wupeny lok kom latin man maber kikore, ce ka wunoŋe ci wudwokka lok, wek an bene acit awore.”</t>
-  </si>
-  <si>
-    <t>I kare ma doŋ guwinyo lok pa kabaka, gucito ki yogi ci guneno lakalatwe ma yam koŋ guneno yo tuŋ wokceŋ ca otelo nyimgi, obino ocuŋ ki malo wa i kabedo ka ma onoŋo latin-nu tye iye</t>
-  </si>
-  <si>
-    <t>Ka guneno lakalatwe meno, cwinygi obedo yom adada.</t>
+    <t>When they had heard the king, they departed; and, lo, the star, which they saw in the east, went before them, till it came and stood over where the young child was.</t>
+  </si>
+  <si>
+    <t>When they saw the star, they rejoiced with exceeding great joy.</t>
+  </si>
+  <si>
+    <t>Gikenyo Herode olwoŋo wendo ma jowok yu Wokchieŋ no i romo ma nyaliŋliŋ, aka oŋeyo kwoŋ jo ndir won ma michala no omenyer'iye ri jo.</t>
+  </si>
+  <si>
+    <t>Gikenyo ooro jo Bethlehem gi wach me: “Kidhi win wirangi kama di nyathi no maber aka ka winwaŋo go wimiyan ŋeyo, ŋey abende abin alam go.”</t>
+  </si>
+  <si>
+    <r>
+      <t>Then Herod summoned the wise men secretly and ascertained from them what time the star had appeared.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> 8 </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>And he sent them to Bethlehem, saying, “Go and search diligently for the child, and when you have found him, bring me word, that I too may come and worship him.”</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>Gi wach me joeye kenyo, aka munyo oido jowotho i royo, joneno michala ma ndir cha joneno yu Wokchieŋ, motelo jo chuka otundo to chungo kama nyathi no oido ni iye.</t>
+  </si>
+  <si>
+    <t>Josangala swa, kendo jowinjo maber moasere munyo joneno michala no!</t>
+  </si>
+  <si>
+    <t>In Bethlehem, i piny pa Yuda,
+iŋati ikiasa thin i dyer jodhum ma Yuda;
+kole kwoŋin ama jatel bino wok'iye,
+ma bino bedo jakwath pa Joisrael.</t>
+  </si>
+  <si>
+    <t>Munyo otyek nywolo Yesu i tindi ma Bethlehem, i Yudeya i ndir ma Herode oido kere, joryeko mogo ma jofuonjere kwoŋ michalin jowok yu Wokchieŋ to jobino Yerusalem aka jopenjo ni, “Nikune nyathi monywol bedo kere pa Joyudaya?"</t>
+  </si>
+  <si>
+    <t>After Jesus was born in Bethlehem in Judea, during the time of King Herod, Magi from the east came to Jerusalemand asked, “Where is the one who has been born king of the Jews? ”</t>
+  </si>
+  <si>
+    <t>We saw his star in the east and have come to worship him.</t>
+  </si>
+  <si>
+    <t>Waneno michala pere munyo owok yu Wokchieŋ amomiyo onyo wabino lamo go.</t>
+  </si>
+  <si>
+    <r>
+      <t>Munyo Kere Herode owinjo gime, obwok, aka kir gi ji man jye i Yerusalem.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Raleway"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>Go olwoŋo jotel pa jochwayi ri Were wi alitar jye kodi jofuonji ma Chik kanyachiel to penjo jo ni, “Ibino nywolo Kristo kune?”</t>
+  </si>
+  <si>
+    <t>Jodwoko ni, “I tindi ma Bethlehem, i Yudeya, me a gima jatuchi wach Were ondiko ” </t>
+  </si>
+  <si>
+    <t>They replied, “In Bethlehem in Judea, for this is what the prophet has written"</t>
+  </si>
+  <si>
+    <t>“ ‘And you, O Bethlehem, in the land of Judah, are by no means least among the rulers of Judah; for from you shall come a ruler who will shepherd my people Israel.’ ”</t>
+  </si>
+  <si>
+    <t>And being warned in a dream not to return to Herod, they departed to their own country by another way.</t>
+  </si>
+  <si>
+    <t>Were onyutho jo i lek nike jokiri jogiki kendo pa Herode, ri ameno jodok yu piny pajo gi royo man.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jodonjo i ot to joneno nyathi bongi Marya yokimere. </t>
+  </si>
+  <si>
+    <t>Joguro chongi gin piny jolamo go, to joyawo migowe pajo, to jochwayo mich: zawabu, buban, kodi mo maŋwe kur.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">And going into the house they saw the child with Mary his mother, and they fell down and worshiped him. </t>
+  </si>
+  <si>
+    <t>Then, opening their treasures, they offered him gifts, gold and frankincense and myrrh.  </t>
+  </si>
+  <si>
+    <t>Munyo jotyeko kadho, malaika pa Ruoth omenyere ri Yozefu i lek munyo wacho ni, “Ayi malo ikwanyi nyathi gi yokimere wiringi i piny Misir, aka wibedi koro nyuka anowachi ri win ndir ma dwoko. Herode lerango nyathi no munyo mito neko.”</t>
+  </si>
+  <si>
+    <t>Now when they had departed, behold, an angel of the Lord appeared to Joseph in a dream and said, “Rise, take the child and his mother, and flee to Egypt, and remain there until I tell you, for Herod is about to search for the child, to destroy him.”</t>
+  </si>
+  <si>
+    <t>Meno omiyo gima jatuchi wach Were owacho chon otundo i kare ni, “Alwoŋo wuodan wok Misir.”</t>
+  </si>
+  <si>
+    <t>Neko nyithindho maŋich</t>
+  </si>
+  <si>
+    <t>Ringo i piny Misir</t>
+  </si>
+  <si>
+    <t>This was to fulfill what the Lord had spoken by the prophet, “Out of Egypt I called my son.”</t>
+  </si>
+  <si>
+    <r>
+      <t>Amomiyo Yozefu oay malo okwanyo nyathi gi yokimere, to joay wor kidho yu Misir;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>kama go obed'iye chuka Herode otho. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>And he rose and took the child and his mother by night and departed to Egypt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> and remained there until the death of Herod. </t>
+    </r>
+  </si>
+  <si>
+    <t>Munyo Herode oneno ni joryeko ma jowok yu Wokchieŋ jothumo ri go ryeko, keme omako go to wodho or nike woneki woko nyithindho mayach jye ma joromo oro aryo gik chien, i Bethlehem kodi loka mothenere gine. </t>
+  </si>
+  <si>
+    <t>Then Herod, when he saw that he had been tricked by the wise men, became furious, and he sent and killed all the male children in Bethlehem and in all that region who were two years old or under.</t>
+  </si>
+  <si>
+    <t>according to the time that he had ascertained from the wise men. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> kwoŋ ndir ma go openj'iye joryeko cha kwoŋ menyirok pa michala.</t>
+  </si>
+  <si>
+    <t>Ameno gima Yeremiya jatuchi wach Were owacho otundo i kare</t>
+  </si>
+  <si>
+    <t>Rakel ywako nyithindho pere.</t>
+  </si>
+  <si>
+    <r>
+      <t>Then was fulfilled what was spoken by the prophet Jeremiah:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Raleway"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>Derino winjere yu Rama, derino ma ywak malith gi ndur.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A voice was heard in Ramah, weeping and loud lamentation, </t>
+  </si>
+  <si>
+    <t>Rachel weeping for her children.</t>
+  </si>
+  <si>
+    <t>Kiyey wokwey chunye, rupiri ongoye modoŋ.</t>
+  </si>
+  <si>
+    <t>She refused to be comforted, because they are no more.</t>
+  </si>
+  <si>
+    <t>The Slaying of the Infants</t>
+  </si>
+  <si>
+    <t>Dwoko wok Misir</t>
+  </si>
+  <si>
+    <t>The flight to Egypt</t>
+  </si>
+  <si>
+    <t>Amomiyo Jozefu oay malo, okwanyo nyathi gi yokimere to jodok yu piny Israel.</t>
+  </si>
+  <si>
+    <r>
+      <t>But when Herod died, behold, an angel of the Lord appeared in a dream to Joseph in Egypt.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Raleway"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>Munyo Herode otyeko tho, malaika pa Ruoth omenyere ri Yozefu i lek yu Misir.</t>
+  </si>
+  <si>
+    <r>
+      <t>And he rose and took the child and his mother and went to the land of Israel.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Raleway"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>Then he said, “Rise, take the child and his mother and go to the land of Israel, for those who sought the child’s life are dead.”</t>
+  </si>
+  <si>
+    <t>Aka owacho ni, “Ayi malo ikwanyi nyathi gi yokimere widoki i piny Israel rupiri joma oido jorango neko go jotyeko tho.”</t>
+  </si>
+  <si>
+    <t>The return from Egypt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Munyo Yozefu owinjo ni Akelayus ama olunjo kom pa bamere Herode paka kere ma Yudeya, lworo omako go dok kendo kenyo. </t>
+  </si>
+  <si>
+    <t>Go otimo ameno ma miyo gima jatuchi wach Were owacho wotundi ni, “Ibino lwoŋo go ni Janazareth.”</t>
+  </si>
+  <si>
+    <t>He did that so  that it might be fulfilled what was spoken by the prophets: “He shall be called a Nazarene.”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To gero pecho pere i tindi ma Nazareth. </t>
+  </si>
+  <si>
+    <t>And he went and lived in a city called Nazareth</t>
+  </si>
+  <si>
+    <t>But when he heard that Archelaus was reigning over Judea in place of his father Herod, he was afraid to go there</t>
+  </si>
+  <si>
+    <t>And being warned in a dream he withdrew to the district of Galilee. </t>
+  </si>
+  <si>
+    <t>Were omedo menyo rigo i lek, amomiyo go okidho i adech ma Galileya </t>
+  </si>
+  <si>
+    <t>Me a bol ma nywolirok pa Yesu Kristo, nyakwar Daudi, nyakwar Ibrayimu</t>
+  </si>
+  <si>
+    <t>Ibrayimu onywolo Isaka, Isaka to nywolo Yakobo, Yakobo to nywolo Yuda gi wutumin go;</t>
+  </si>
+  <si>
+    <t>Abraham was the father of Isaac, and Isaac the father of Jacob, and Jacob the father of Judah and his brothers</t>
+  </si>
+  <si>
+    <t>Yakobo to nywolo Yozefu, mobedo chwor Marya, monywolo Yesu milwoŋo ni Kristo.</t>
+  </si>
+  <si>
+    <r>
+      <t>Jacob fathered Joseph the husband of Mary, of whom Jesus was born, who is called Christ.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Raleway"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>Ri ameno, wok kwoŋ Ibrayimu tundo kwoŋi Daudi, obedo luse ji apar g'aŋwen; odoko wok kwoŋ Daudi, tundo munyo oter jo yu Babilon, obedo luse ji apar gaŋwen; kendo wok munyo oter jo yu Babilon tundo kwoŋ Kristo, bende obedo luse ji apar g'aŋwen.</t>
+  </si>
+  <si>
+    <t>So all the generations from Abraham to David were fourteen generations, and from David to the deportation to Babylon fourteen generations, and from the deportation to Babylon to the Christ fourteen generations.</t>
+  </si>
+  <si>
+    <t>The birth of Jesus</t>
+  </si>
+  <si>
+    <t>Nywolirok pa Yesu Kristo</t>
+  </si>
+  <si>
+    <t>Now the birth of Jesus Christ took place in this way. When his mother Mary had been betrothed to Joseph, before they came together she was found to be with child from the Holy Spirit.</t>
+  </si>
+  <si>
+    <t>Gikenyo Yozefu chwore, rupiri oido obedo dhano motire aka komito miyo go wichkwot, oido paro weyo go nyaliŋliŋ.</t>
+  </si>
+  <si>
+    <t> Neni, munyo fuodi go paro ameno, malaika pa Ruoth to bino ri go i lek, to wacho ri go ni, “Yozefu wuodi pa Daudi, ikiri ilwor rwako Marya bedo dhako perin, rupiri go yach gi men pa Chuny Maleŋ.</t>
+  </si>
+  <si>
+    <r>
+      <t>Me apaka nywolirok pa Yesu Kristo obedo: Munyo Yozefu fuodi oido nyaka jochikere nywomirok kodi Marya min Yesu, ma fuodi korwako go i ot, to nenere ni go oido otyeko gamo iye i men pa Chuny Maleŋ.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Raleway"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>And her husband Joseph, being a just man and unwilling to put her to shame, resolved to divorce her quietly.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Raleway"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>But as he considered these things, behold, an angel of the Lord appeared to him in a dream, saying, “Joseph, son of David, do not fear to take Mary as your wife, for that which is conceived in her is from the Holy Spirit.</t>
+  </si>
+  <si>
+    <r>
+      <t>Go bino nywolo nyathi ma jayach, aka ibino chwoko nyinge ni Yesu; rupiri go ama bino botho ji pere kwoŋ recho pajo.”</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Raleway"/>
+      </rPr>
+      <t>  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FF000000"/>
+        <rFont val="Raleway"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>She will bear a son, and you shall call his name Jesus, for he will save his people from their sins.”</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Raleway"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>Nyako ma fuodi kuya jachwo bino gamo iye, to nywolo nyathi ma jayach, ma ibino chwoko nyinge ni “Emanwel”,dwoŋ mere ni, “Were ni gi wan.” </t>
+  </si>
+  <si>
+    <t> Behold, the virgin shall conceive and bear a son, and they shall call his name “Immanuel” which means, “ God with us.”  </t>
+  </si>
+  <si>
+    <t>Gino jye otimere, ŋey gima jatuchi wach Were oluwo wotundi i kare </t>
+  </si>
+  <si>
+    <t> All this took place to fulfill what the Lord had spoken by the prophet</t>
+  </si>
+  <si>
+    <t>Yozefu munyo ochiew, to timo paka malaika pa Were owacho ri go, to tero Marya bedo chiege.</t>
+  </si>
+  <si>
+    <t>When Joseph woke from sleep, he did as the angel of the Lord commanded him: he took his wife.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aka koŋeyere gine tundo munyo ochowo nywolo nyathi no </t>
+  </si>
+  <si>
+    <t>to chwoko nyinge ni Yesu.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">but knew her not until she had given birth to a son </t>
+  </si>
+  <si>
+    <t>And he called his name Jesus.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,6 +490,32 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="17"/>
+      <color rgb="FF000000"/>
+      <name val="Raleway"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Raleway"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -116,12 +547,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -418,16 +855,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="65.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="53.42578125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="65.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="53.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -438,88 +875,507 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30">
       <c r="A2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30">
+      <c r="A3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="30.75">
+      <c r="A4" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4">
+        <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="75">
+      <c r="A5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5">
+        <v>1.17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6">
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="60">
+      <c r="A7" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7">
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30.75">
+      <c r="A8" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8">
+        <v>1.19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="60">
+      <c r="A9" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30.75">
+      <c r="A10" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10">
+        <v>1.21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30">
+      <c r="A11" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="45">
+      <c r="A12" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="30">
+      <c r="A13" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C14">
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15">
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="60">
+      <c r="A16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30">
+      <c r="A17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="30.75">
+      <c r="A18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="75">
-      <c r="A3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="C18">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="45">
+      <c r="A19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="30">
-      <c r="A4" s="2" t="s">
+      <c r="C19">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30">
+      <c r="A20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="60">
+      <c r="A21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="45">
+      <c r="A22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="45">
+      <c r="A23" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="45">
+      <c r="A24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="45">
-      <c r="A5" s="2" t="s">
+      <c r="C24">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="30">
+      <c r="A25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="30">
-      <c r="A6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="30">
-      <c r="A7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7">
-        <v>2.7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="45">
-      <c r="A8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8">
-        <v>2.8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="45">
-      <c r="A9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9">
-        <v>2.9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="2" t="s">
-        <v>16</v>
+      <c r="C25">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="30">
+      <c r="A26" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26">
+        <v>2.11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="30">
+      <c r="A27" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27">
+        <v>2.11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="30">
+      <c r="A28" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28">
+        <v>2.12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="75">
+      <c r="A29" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29">
+        <v>2.13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="45">
+      <c r="A30" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30">
+        <v>2.14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="30">
+      <c r="A31" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32">
+        <v>2.16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33">
+        <v>2.13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="60">
+      <c r="A34" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34">
+        <v>2.16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="30">
+      <c r="A35" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35">
+        <v>2.16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="30.75">
+      <c r="A36" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36">
+        <v>2.17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="30">
+      <c r="A37" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37">
+        <v>2.1800000000000002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38">
+        <v>2.1800000000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="30.75">
+      <c r="A41" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C41">
+        <v>2.19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="45">
+      <c r="A42" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C42">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="30.75">
+      <c r="A43" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C43">
+        <v>2.21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="45">
+      <c r="A44" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C44">
+        <v>2.2200000000000002</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="30">
+      <c r="A45" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C45">
+        <v>2.2200000000000002</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C46">
+        <v>2.23</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="30">
+      <c r="A47" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C47">
+        <v>2.23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished with the storybooks
</commit_message>
<xml_diff>
--- a/Bible - NT.xlsx
+++ b/Bible - NT.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Mathew" sheetId="1" r:id="rId1"/>
@@ -3109,8 +3109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C267"/>
   <sheetViews>
-    <sheetView topLeftCell="A258" workbookViewId="0">
-      <selection activeCell="B267" sqref="B267"/>
+    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="A130" sqref="A130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6029,7 +6029,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -6038,7 +6038,7 @@
     <col min="1" max="1" width="46" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="45">
+    <row r="1" spans="1:1">
       <c r="A1" s="2" t="s">
         <v>520</v>
       </c>

</xml_diff>